<commit_message>
Update DpdkFunctions page in spreadsheet
Signed-off-by: Derek Foster <derek.foster@intel.com>
</commit_message>
<xml_diff>
--- a/ovs-p4rt/sidecar/tests/FunctionsWithTests.xlsx
+++ b/ovs-p4rt/sidecar/tests/FunctionsWithTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BDDF76-1C91-43F2-AD1D-10528CC7C6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE59C27-2156-4A9D-AC31-41C81EBA1378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8745" yWindow="5490" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
   <si>
     <t>PrepareDstIpMacMapTableEntry</t>
   </si>
@@ -334,13 +334,19 @@
   </si>
   <si>
     <t>dpdk_vxlan_encap_test</t>
+  </si>
+  <si>
+    <t>l2_fwd_rx_with_tunnel_table</t>
+  </si>
+  <si>
+    <t>dpdk_fdb_tx_vlan_test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +487,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008080"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -669,7 +695,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -844,6 +870,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -889,7 +928,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -900,10 +939,23 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1288,7 +1340,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -1297,7 +1349,7 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -1314,7 +1366,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1331,7 +1383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1348,7 +1400,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1434,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1399,7 +1451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1416,7 +1468,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1485,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1450,7 +1502,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1519,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1484,7 +1536,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1501,7 +1553,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1518,7 +1570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1535,7 +1587,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1604,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1569,7 +1621,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1586,7 +1638,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1603,7 +1655,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1620,7 +1672,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1637,7 +1689,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1654,7 +1706,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1671,7 +1723,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1688,7 +1740,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1705,7 +1757,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1722,7 +1774,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1739,7 +1791,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -1756,7 +1808,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1773,7 +1825,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -1790,7 +1842,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
@@ -1822,17 +1874,17 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -1849,31 +1901,31 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1883,12 +1935,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>39</v>
+      <c r="B4" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>44</v>
@@ -1900,11 +1952,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="16" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1917,11 +1969,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="17" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1934,11 +1986,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="18" t="s">
         <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1951,11 +2003,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="19" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1968,11 +2020,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1985,11 +2037,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="20" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1998,7 +2050,7 @@
       <c r="D10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ovsp4rt] Updated FunctionsWithTests spreadsheet
Signed-off-by: Derek Foster <derek.foster@intel.com>
</commit_message>
<xml_diff>
--- a/ovs-p4rt/sidecar/tests/FunctionsWithTests.xlsx
+++ b/ovs-p4rt/sidecar/tests/FunctionsWithTests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE59C27-2156-4A9D-AC31-41C81EBA1378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBC1DD-3BFB-4A9C-84A8-82C64275305B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="5490" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
   </bookViews>
   <sheets>
     <sheet name="ES2K Functions" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="104">
   <si>
     <t>PrepareDstIpMacMapTableEntry</t>
   </si>
@@ -315,22 +315,10 @@
     <t>dpdk_fdb_rx_vlan_test</t>
   </si>
   <si>
-    <t>dpdk_fdb_tx_geneve_test</t>
-  </si>
-  <si>
     <t>dpdk_fdb_tx_vxlan_test</t>
   </si>
   <si>
-    <t>dpdk_geneve_decap_test</t>
-  </si>
-  <si>
-    <t>dpdk_geneve_encap_test</t>
-  </si>
-  <si>
     <t>dpdk_tunnel_term_test</t>
-  </si>
-  <si>
-    <t>dpdk_vxlan_decap_test</t>
   </si>
   <si>
     <t>dpdk_vxlan_encap_test</t>
@@ -346,7 +334,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,26 +475,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF008080"/>
-      <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -695,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -870,19 +838,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -928,7 +883,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -936,26 +891,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1340,7 +1279,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
@@ -1349,7 +1288,7 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -1366,7 +1305,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1322,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1339,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1417,7 +1356,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1434,7 +1373,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1451,7 +1390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1407,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1485,7 +1424,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1519,7 +1458,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1536,7 +1475,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1553,7 +1492,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1509,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1587,7 +1526,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1604,7 +1543,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1621,7 +1560,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1577,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1655,7 +1594,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1672,7 +1611,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1689,7 +1628,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1706,7 +1645,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1723,7 +1662,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1740,7 +1679,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1757,7 +1696,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1713,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1791,7 +1730,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -1808,7 +1747,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1825,7 +1764,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -1842,7 +1781,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
@@ -1871,20 +1810,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEB699C-3EA8-4859-9609-A503AFBC82B9}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -1901,31 +1840,31 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="E2" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1935,12 +1874,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>107</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>44</v>
@@ -1952,106 +1891,38 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>97</v>
+      <c r="E6" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>